<commit_message>
Added model ROS to code and to excel sheet
</commit_message>
<xml_diff>
--- a/ROS_calculations.xlsx
+++ b/ROS_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/Hill_Runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E72ED4F-7B27-9346-B843-F61ECE2C3B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97708F86-81C9-8145-AC29-36CBC87D94A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="17280" windowHeight="21700" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>ROS Data</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Run_21</t>
+  </si>
+  <si>
+    <t>Model ROS</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C5D8E9-26BC-FC46-9670-57C49E39CB3F}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,376 +755,556 @@
         <v>0.62129999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>10.511709</v>
-      </c>
-      <c r="C7">
-        <v>10.606191000000001</v>
-      </c>
-      <c r="D7">
-        <v>10.183984000000001</v>
-      </c>
-      <c r="E7">
-        <v>10.512212</v>
-      </c>
-      <c r="F7">
-        <v>10.121859000000001</v>
-      </c>
-      <c r="G7">
-        <v>10.623476999999999</v>
-      </c>
-      <c r="I7">
-        <v>10.512638000000001</v>
-      </c>
-      <c r="K7">
-        <v>10.546491</v>
-      </c>
-      <c r="L7">
-        <v>10.453250000000001</v>
-      </c>
-      <c r="M7">
-        <v>10.512064000000001</v>
-      </c>
-      <c r="N7">
-        <v>10.442306500000001</v>
-      </c>
-      <c r="O7">
-        <v>10.476487000000001</v>
-      </c>
-      <c r="P7">
-        <v>10.4758</v>
-      </c>
-      <c r="Q7">
-        <v>10.511231</v>
-      </c>
-      <c r="R7">
-        <v>10.455652000000001</v>
-      </c>
-      <c r="S7">
-        <v>10.511894</v>
-      </c>
-      <c r="T7">
-        <v>10.511896</v>
-      </c>
-      <c r="U7">
-        <v>10.511658000000001</v>
-      </c>
-      <c r="V7">
-        <v>10.511988000000001</v>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>2.3831376999999998</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>1.9875708000000001</v>
+      </c>
+      <c r="G6">
+        <v>5.0585839999999997</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>6.0000004999999996</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <v>6.0000004999999996</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <v>6.0000004999999996</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.29007253</v>
+        <v>10.511709</v>
       </c>
       <c r="C8">
-        <v>0.29007253</v>
+        <v>10.606191000000001</v>
       </c>
       <c r="D8">
-        <v>0.29007253</v>
+        <v>10.183984000000001</v>
       </c>
       <c r="E8">
-        <v>0.29007253</v>
+        <v>10.512212</v>
       </c>
       <c r="F8">
-        <v>0.29007253</v>
+        <v>10.121859000000001</v>
       </c>
       <c r="G8">
-        <v>0.29007253</v>
-      </c>
-      <c r="H8">
-        <v>0.29007253</v>
+        <v>10.623476999999999</v>
       </c>
       <c r="I8">
-        <v>0.29007253</v>
-      </c>
-      <c r="J8">
-        <v>0.29007253</v>
+        <v>10.512638000000001</v>
       </c>
       <c r="K8">
-        <v>0.29007253</v>
+        <v>10.546491</v>
       </c>
       <c r="L8">
-        <v>0.29007253</v>
+        <v>10.453250000000001</v>
       </c>
       <c r="M8">
-        <v>0.29007253</v>
+        <v>10.512064000000001</v>
       </c>
       <c r="N8">
-        <v>0.29007253</v>
+        <v>10.442306500000001</v>
       </c>
       <c r="O8">
-        <v>0.29007253</v>
+        <v>10.476487000000001</v>
       </c>
       <c r="P8">
-        <v>0.29007253</v>
+        <v>10.4758</v>
       </c>
       <c r="Q8">
-        <v>0.29007253</v>
+        <v>10.511231</v>
       </c>
       <c r="R8">
-        <v>0.29007253</v>
+        <v>10.455652000000001</v>
       </c>
       <c r="S8">
-        <v>0.29007253</v>
+        <v>10.511894</v>
       </c>
       <c r="T8">
-        <v>0.29007253</v>
+        <v>10.511896</v>
       </c>
       <c r="U8">
-        <v>0.29007253</v>
+        <v>10.511658000000001</v>
       </c>
       <c r="V8">
-        <v>0.29007253</v>
+        <v>10.511988000000001</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.29007253</v>
+      </c>
+      <c r="C9">
+        <v>0.29007253</v>
+      </c>
+      <c r="D9">
+        <v>0.29007253</v>
+      </c>
+      <c r="E9">
+        <v>0.29007253</v>
+      </c>
+      <c r="F9">
+        <v>0.29007253</v>
+      </c>
+      <c r="G9">
+        <v>0.29007253</v>
+      </c>
+      <c r="H9">
+        <v>0.29007253</v>
+      </c>
+      <c r="I9">
+        <v>0.29007253</v>
+      </c>
+      <c r="J9">
+        <v>0.29007253</v>
+      </c>
+      <c r="K9">
+        <v>0.29007253</v>
+      </c>
+      <c r="L9">
+        <v>0.29007253</v>
+      </c>
+      <c r="M9">
+        <v>0.29007253</v>
+      </c>
+      <c r="N9">
+        <v>0.29007253</v>
+      </c>
+      <c r="O9">
+        <v>0.29007253</v>
+      </c>
+      <c r="P9">
+        <v>0.29007253</v>
+      </c>
+      <c r="Q9">
+        <v>0.29007253</v>
+      </c>
+      <c r="R9">
+        <v>0.29007253</v>
+      </c>
+      <c r="S9">
+        <v>0.29007253</v>
+      </c>
+      <c r="T9">
+        <v>0.29007253</v>
+      </c>
+      <c r="U9">
+        <v>0.29007253</v>
+      </c>
+      <c r="V9">
+        <v>0.29007253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>0.4864</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>0.4899</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>0.47410000000000002</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>0.4864</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>0.4718</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>0.49059999999999998</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>0.4864</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>0.48770000000000002</v>
       </c>
-      <c r="L9">
+      <c r="L10">
         <v>0.48770000000000002</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>0.4864</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>0.48380000000000001</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>10.476487000000001</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>0.48499999999999999</v>
       </c>
-      <c r="Q9">
+      <c r="Q10">
         <v>0.4864</v>
       </c>
-      <c r="R9">
+      <c r="R10">
         <v>0.48430000000000001</v>
       </c>
-      <c r="S9">
+      <c r="S10">
         <v>0.4864</v>
       </c>
-      <c r="T9">
+      <c r="T10">
         <v>0.4864</v>
       </c>
-      <c r="U9">
+      <c r="U10">
         <v>0.4864</v>
       </c>
-      <c r="V9">
+      <c r="V10">
         <v>10.511988000000001</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>10.088276</v>
+        <v>0.60530806000000004</v>
       </c>
       <c r="C11">
-        <v>10.172914499999999</v>
+        <v>0.60672959999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.40722406</v>
       </c>
       <c r="E11">
-        <v>10.088552</v>
+        <v>0.60585829999999996</v>
+      </c>
+      <c r="F11">
+        <v>0.38986418</v>
       </c>
       <c r="G11">
-        <v>10.184378000000001</v>
+        <v>0.62131625000000001</v>
       </c>
       <c r="I11">
-        <v>10.088162000000001</v>
+        <v>0.60610549999999996</v>
       </c>
       <c r="K11">
-        <v>10.125124</v>
+        <v>0.61175597000000004</v>
       </c>
       <c r="L11">
-        <v>9.9728750000000002</v>
+        <v>0.52608319999999997</v>
       </c>
       <c r="M11">
-        <v>10.088305999999999</v>
+        <v>0.60557395000000003</v>
       </c>
       <c r="N11">
-        <v>10.026384</v>
+        <v>0.51828969999999996</v>
       </c>
       <c r="O11">
-        <v>10.053661999999999</v>
+        <v>0.60281085999999995</v>
       </c>
       <c r="P11">
-        <v>10.116463</v>
+        <v>0.60864339999999995</v>
       </c>
       <c r="Q11">
-        <v>10.088471999999999</v>
+        <v>0.60507619999999995</v>
       </c>
       <c r="R11">
-        <v>10.095207</v>
+        <v>0.60420436</v>
       </c>
       <c r="S11">
-        <v>10.088437000000001</v>
+        <v>0.60536160000000006</v>
       </c>
       <c r="T11">
-        <v>10.088939</v>
+        <v>0.60522880000000001</v>
       </c>
       <c r="U11">
-        <v>10.088243</v>
+        <v>0.6053636</v>
       </c>
       <c r="V11">
-        <v>10.089027</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0.34060466</v>
-      </c>
-      <c r="C12">
-        <v>0.34060466</v>
-      </c>
-      <c r="D12">
-        <v>0.34060466</v>
-      </c>
-      <c r="E12">
-        <v>0.34060466</v>
-      </c>
-      <c r="F12">
-        <v>0.34060466</v>
-      </c>
-      <c r="G12">
-        <v>0.34060466</v>
-      </c>
-      <c r="H12">
-        <v>0.34060466</v>
-      </c>
-      <c r="I12">
-        <v>0.34060466</v>
-      </c>
-      <c r="J12">
-        <v>0.34060466</v>
-      </c>
-      <c r="K12">
-        <v>0.34060466</v>
-      </c>
-      <c r="L12">
-        <v>0.34060466</v>
-      </c>
-      <c r="M12">
-        <v>0.34060466</v>
-      </c>
-      <c r="N12">
-        <v>0.34060466</v>
-      </c>
-      <c r="O12">
-        <v>0.34060466</v>
-      </c>
-      <c r="P12">
-        <v>0.34060466</v>
-      </c>
-      <c r="Q12">
-        <v>0.34060466</v>
-      </c>
-      <c r="R12">
-        <v>0.34060466</v>
-      </c>
-      <c r="S12">
-        <v>0.34060466</v>
-      </c>
-      <c r="T12">
-        <v>0.34060466</v>
-      </c>
-      <c r="U12">
-        <v>0.34060466</v>
-      </c>
-      <c r="V12">
-        <v>0.34060466</v>
+        <v>0.60534980000000005</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>10.088276</v>
+      </c>
+      <c r="C13">
+        <v>10.172914499999999</v>
+      </c>
+      <c r="E13">
+        <v>10.088552</v>
+      </c>
+      <c r="G13">
+        <v>10.184378000000001</v>
+      </c>
+      <c r="I13">
+        <v>10.088162000000001</v>
+      </c>
+      <c r="K13">
+        <v>10.125124</v>
+      </c>
+      <c r="L13">
+        <v>9.9728750000000002</v>
+      </c>
+      <c r="M13">
+        <v>10.088305999999999</v>
+      </c>
+      <c r="N13">
+        <v>10.026384</v>
+      </c>
+      <c r="O13">
+        <v>10.053661999999999</v>
+      </c>
+      <c r="P13">
+        <v>10.116463</v>
+      </c>
+      <c r="Q13">
+        <v>10.088471999999999</v>
+      </c>
+      <c r="R13">
+        <v>10.095207</v>
+      </c>
+      <c r="S13">
+        <v>10.088437000000001</v>
+      </c>
+      <c r="T13">
+        <v>10.088939</v>
+      </c>
+      <c r="U13">
+        <v>10.088243</v>
+      </c>
+      <c r="V13">
+        <v>10.089027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0.34060466</v>
+      </c>
+      <c r="C14">
+        <v>0.34060466</v>
+      </c>
+      <c r="D14">
+        <v>0.34060466</v>
+      </c>
+      <c r="E14">
+        <v>0.34060466</v>
+      </c>
+      <c r="F14">
+        <v>0.34060466</v>
+      </c>
+      <c r="G14">
+        <v>0.34060466</v>
+      </c>
+      <c r="H14">
+        <v>0.34060466</v>
+      </c>
+      <c r="I14">
+        <v>0.34060466</v>
+      </c>
+      <c r="J14">
+        <v>0.34060466</v>
+      </c>
+      <c r="K14">
+        <v>0.34060466</v>
+      </c>
+      <c r="L14">
+        <v>0.34060466</v>
+      </c>
+      <c r="M14">
+        <v>0.34060466</v>
+      </c>
+      <c r="N14">
+        <v>0.34060466</v>
+      </c>
+      <c r="O14">
+        <v>0.34060466</v>
+      </c>
+      <c r="P14">
+        <v>0.34060466</v>
+      </c>
+      <c r="Q14">
+        <v>0.34060466</v>
+      </c>
+      <c r="R14">
+        <v>0.34060466</v>
+      </c>
+      <c r="S14">
+        <v>0.34060466</v>
+      </c>
+      <c r="T14">
+        <v>0.34060466</v>
+      </c>
+      <c r="U14">
+        <v>0.34060466</v>
+      </c>
+      <c r="V14">
+        <v>0.34060466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="C13">
-        <v>0.34060466</v>
-      </c>
-      <c r="E13">
+      <c r="C15">
+        <v>0.34060466</v>
+      </c>
+      <c r="E15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.4884</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="K13">
+      <c r="K15">
         <v>0.48620000000000002</v>
       </c>
-      <c r="L13">
+      <c r="L15">
         <v>0.48049999999999998</v>
       </c>
-      <c r="M13">
+      <c r="M15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="N13">
+      <c r="N15">
         <v>0.48249999999999998</v>
       </c>
-      <c r="O13">
+      <c r="O15">
         <v>0.48349999999999999</v>
       </c>
-      <c r="P13">
+      <c r="P15">
         <v>0.4859</v>
       </c>
-      <c r="Q13">
+      <c r="Q15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="R13">
+      <c r="R15">
         <v>0.48509999999999998</v>
       </c>
-      <c r="S13">
+      <c r="S15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="T13">
+      <c r="T15">
         <v>0.4849</v>
       </c>
-      <c r="U13">
+      <c r="U15">
         <v>0.48480000000000001</v>
       </c>
-      <c r="V13">
+      <c r="V15">
         <v>0.4849</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>0.68085600000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.64096624000000002</v>
+      </c>
+      <c r="E16">
+        <v>0.6803785</v>
+      </c>
+      <c r="G16">
+        <v>0.60257470000000002</v>
+      </c>
+      <c r="I16">
+        <v>0.68052029999999997</v>
+      </c>
+      <c r="K16">
+        <v>0.65760960000000002</v>
+      </c>
+      <c r="L16">
+        <v>0.62494479999999997</v>
+      </c>
+      <c r="M16">
+        <v>0.68055220000000005</v>
+      </c>
+      <c r="N16">
+        <v>0.60391843000000001</v>
+      </c>
+      <c r="O16">
+        <v>0.67636067</v>
+      </c>
+      <c r="P16">
+        <v>0.78299266000000001</v>
+      </c>
+      <c r="Q16">
+        <v>0.68069259999999998</v>
+      </c>
+      <c r="R16">
+        <v>0.75873279999999999</v>
+      </c>
+      <c r="S16">
+        <v>0.68084513999999996</v>
+      </c>
+      <c r="T16">
+        <v>0.67894129999999997</v>
+      </c>
+      <c r="U16">
+        <v>0.68056333000000002</v>
+      </c>
+      <c r="V16">
+        <v>0.67868139999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new code and calculating new ROS
</commit_message>
<xml_diff>
--- a/ROS_calculations.xlsx
+++ b/ROS_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/Hill_Runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DEE6A2-E0FB-654B-8612-B93A6A4B0240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E643DD7-2E8F-AA4C-A441-ED1512431DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
+    <workbookView xWindow="17280" yWindow="640" windowWidth="17280" windowHeight="21700" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>ROS Data</t>
   </si>
@@ -131,19 +131,46 @@
   </si>
   <si>
     <t>Model ROS</t>
+  </si>
+  <si>
+    <t>adjr0</t>
+  </si>
+  <si>
+    <t>adjrw</t>
+  </si>
+  <si>
+    <t>adjrs</t>
+  </si>
+  <si>
+    <t>Modified Rothermel Matlab Code</t>
+  </si>
+  <si>
+    <t>Original Rothermel Matlab Code</t>
+  </si>
+  <si>
+    <t>ROS var modified</t>
+  </si>
+  <si>
+    <t>ROS var original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,8 +193,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C5D8E9-26BC-FC46-9670-57C49E39CB3F}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,813 +527,1471 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" t="s">
-        <v>30</v>
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.25</v>
+      </c>
+      <c r="J2">
+        <v>0.25</v>
+      </c>
+      <c r="K2">
+        <v>0.75</v>
+      </c>
+      <c r="N2">
+        <v>0.75</v>
+      </c>
+      <c r="O2">
+        <v>1.25</v>
+      </c>
+      <c r="R2">
+        <v>1.25</v>
+      </c>
+      <c r="S2">
+        <v>0.999</v>
+      </c>
+      <c r="V2">
+        <v>0.999</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>15.979096</v>
-      </c>
-      <c r="C3">
-        <v>15.979676</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>14.204286</v>
-      </c>
-      <c r="E3">
-        <v>15.985248</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>13.884665500000001</v>
-      </c>
-      <c r="G3">
-        <v>15.94369</v>
-      </c>
-      <c r="I3">
-        <v>15.988474999999999</v>
-      </c>
-      <c r="K3">
-        <v>16.009450000000001</v>
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>0.25</v>
+      </c>
+      <c r="J3">
+        <v>0.25</v>
       </c>
       <c r="L3">
-        <v>15.592441000000001</v>
-      </c>
-      <c r="M3">
-        <v>15.98211</v>
+        <v>0.75</v>
       </c>
       <c r="N3">
-        <v>15.435043</v>
-      </c>
-      <c r="O3">
-        <v>16.008780000000002</v>
+        <v>0.75</v>
       </c>
       <c r="P3">
-        <v>16.254318000000001</v>
-      </c>
-      <c r="Q3">
-        <v>15.975887999999999</v>
+        <v>1.25</v>
       </c>
       <c r="R3">
-        <v>16.241644000000001</v>
-      </c>
-      <c r="S3">
-        <v>15.979746</v>
+        <v>1.25</v>
       </c>
       <c r="T3">
-        <v>15.981907</v>
-      </c>
-      <c r="U3">
-        <v>15.979161</v>
+        <v>0.999</v>
       </c>
       <c r="V3">
-        <v>15.982637</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="C4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="D4">
-        <v>3.9121687000000002E-2</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="G4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="H4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.25</v>
       </c>
       <c r="J4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="K4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="L4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.25</v>
       </c>
       <c r="M4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.75</v>
       </c>
       <c r="N4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="O4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="P4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.75</v>
       </c>
       <c r="Q4">
-        <v>3.9121687000000002E-2</v>
+        <v>1.25</v>
       </c>
       <c r="R4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="S4">
-        <v>3.9121687000000002E-2</v>
-      </c>
-      <c r="T4">
-        <v>3.9121687000000002E-2</v>
+        <v>1.25</v>
       </c>
       <c r="U4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.999</v>
       </c>
       <c r="V4">
-        <v>3.9121687000000002E-2</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.62119999999999997</v>
-      </c>
-      <c r="C5">
-        <v>0.62119999999999997</v>
-      </c>
-      <c r="D5">
-        <v>0.55379999999999996</v>
-      </c>
-      <c r="E5">
-        <v>0.62139999999999995</v>
-      </c>
-      <c r="F5">
-        <v>0.54179999999999995</v>
-      </c>
-      <c r="G5">
-        <v>0.61980000000000002</v>
-      </c>
-      <c r="I5">
-        <v>0.62150000000000005</v>
-      </c>
-      <c r="K5">
-        <v>0.62229999999999996</v>
-      </c>
-      <c r="L5">
-        <v>0.60640000000000005</v>
-      </c>
-      <c r="M5">
-        <v>0.62129999999999996</v>
-      </c>
-      <c r="N5">
-        <v>0.60050000000000003</v>
-      </c>
-      <c r="O5">
-        <v>0.62229999999999996</v>
-      </c>
-      <c r="P5">
-        <v>0.63160000000000005</v>
-      </c>
-      <c r="Q5">
-        <v>0.621</v>
-      </c>
-      <c r="R5">
-        <v>0.63119999999999998</v>
-      </c>
-      <c r="S5">
-        <v>0.62119999999999997</v>
-      </c>
-      <c r="T5">
-        <v>0.62129999999999996</v>
-      </c>
-      <c r="U5">
-        <v>0.62119999999999997</v>
-      </c>
-      <c r="V5">
-        <v>0.62129999999999996</v>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>15.979096</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>15.979676</v>
       </c>
       <c r="D6">
-        <v>2.3831376999999998</v>
+        <v>14.204286</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>15.985248</v>
       </c>
       <c r="F6">
-        <v>1.9875708000000001</v>
+        <v>13.884665500000001</v>
       </c>
       <c r="G6">
-        <v>5.0585839999999997</v>
+        <v>15.94369</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>15.988474999999999</v>
       </c>
       <c r="K6">
-        <v>6.0000004999999996</v>
+        <v>16.009450000000001</v>
       </c>
       <c r="L6">
-        <v>6</v>
+        <v>15.592441000000001</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>15.98211</v>
       </c>
       <c r="N6">
-        <v>6</v>
+        <v>15.435043</v>
       </c>
       <c r="O6">
-        <v>6</v>
+        <v>16.008780000000002</v>
       </c>
       <c r="P6">
-        <v>6</v>
+        <v>16.254318000000001</v>
       </c>
       <c r="Q6">
-        <v>6</v>
+        <v>15.975887999999999</v>
       </c>
       <c r="R6">
-        <v>6</v>
+        <v>16.241644000000001</v>
       </c>
       <c r="S6">
-        <v>6.0000004999999996</v>
+        <v>15.979746</v>
       </c>
       <c r="T6">
-        <v>6</v>
+        <v>15.981907</v>
       </c>
       <c r="U6">
-        <v>6</v>
+        <v>15.979161</v>
       </c>
       <c r="V6">
-        <v>6.0000004999999996</v>
+        <v>15.982637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="F7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="G7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="H7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="I7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="K7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="L7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="M7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="N7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="O7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="P7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="Q7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="R7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="S7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="T7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="U7">
+        <v>3.9121687000000002E-2</v>
+      </c>
+      <c r="V7">
+        <v>3.9121687000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>10.511709</v>
+        <v>0.62119999999999997</v>
       </c>
       <c r="C8">
-        <v>10.606191000000001</v>
+        <v>0.62119999999999997</v>
       </c>
       <c r="D8">
-        <v>10.183984000000001</v>
+        <v>0.55379999999999996</v>
       </c>
       <c r="E8">
-        <v>10.512212</v>
+        <v>0.62139999999999995</v>
       </c>
       <c r="F8">
-        <v>10.121859000000001</v>
+        <v>0.54179999999999995</v>
       </c>
       <c r="G8">
-        <v>10.623476999999999</v>
+        <v>0.61980000000000002</v>
       </c>
       <c r="I8">
-        <v>10.512638000000001</v>
+        <v>0.62150000000000005</v>
       </c>
       <c r="K8">
-        <v>10.546491</v>
+        <v>0.62229999999999996</v>
       </c>
       <c r="L8">
-        <v>10.453250000000001</v>
+        <v>0.60640000000000005</v>
       </c>
       <c r="M8">
-        <v>10.512064000000001</v>
+        <v>0.62129999999999996</v>
       </c>
       <c r="N8">
-        <v>10.442306500000001</v>
+        <v>0.60050000000000003</v>
       </c>
       <c r="O8">
-        <v>10.476487000000001</v>
+        <v>0.62229999999999996</v>
       </c>
       <c r="P8">
-        <v>10.4758</v>
+        <v>0.63160000000000005</v>
       </c>
       <c r="Q8">
-        <v>10.511231</v>
+        <v>0.621</v>
       </c>
       <c r="R8">
-        <v>10.455652000000001</v>
+        <v>0.63119999999999998</v>
       </c>
       <c r="S8">
-        <v>10.511894</v>
+        <v>0.62119999999999997</v>
       </c>
       <c r="T8">
-        <v>10.511896</v>
+        <v>0.62129999999999996</v>
       </c>
       <c r="U8">
-        <v>10.511658000000001</v>
+        <v>0.62119999999999997</v>
       </c>
       <c r="V8">
-        <v>10.511988000000001</v>
+        <v>0.62129999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>0.29007253</v>
+        <v>2.3831376999999998</v>
       </c>
       <c r="E9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>0.29007253</v>
+        <v>1.9875708000000001</v>
       </c>
       <c r="G9">
-        <v>0.29007253</v>
-      </c>
-      <c r="H9">
-        <v>0.29007253</v>
+        <v>5.0585839999999997</v>
       </c>
       <c r="I9">
-        <v>0.29007253</v>
-      </c>
-      <c r="J9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="K9">
-        <v>0.29007253</v>
+        <v>6.0000004999999996</v>
       </c>
       <c r="L9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="M9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="N9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="O9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="P9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="Q9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="R9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="S9">
-        <v>0.29007253</v>
+        <v>6.0000004999999996</v>
       </c>
       <c r="T9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="U9">
-        <v>0.29007253</v>
+        <v>6</v>
       </c>
       <c r="V9">
-        <v>0.29007253</v>
+        <v>6.0000004999999996</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>0.4899</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>0.47410000000000002</v>
+        <v>4.9615</v>
       </c>
       <c r="E10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>0.4718</v>
+        <v>4.7991000000000001</v>
       </c>
       <c r="G10">
-        <v>0.49059999999999998</v>
+        <v>6</v>
       </c>
       <c r="I10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="K10">
-        <v>0.48770000000000002</v>
+        <v>6</v>
       </c>
       <c r="L10">
-        <v>0.48770000000000002</v>
+        <v>6</v>
       </c>
       <c r="M10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="N10">
-        <v>0.48380000000000001</v>
+        <v>6</v>
       </c>
       <c r="O10">
-        <v>10.476487000000001</v>
+        <v>6</v>
       </c>
       <c r="P10">
-        <v>0.48499999999999999</v>
+        <v>6</v>
       </c>
       <c r="Q10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="R10">
-        <v>0.48430000000000001</v>
+        <v>6</v>
       </c>
       <c r="S10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="T10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="U10">
-        <v>0.4864</v>
+        <v>6</v>
       </c>
       <c r="V10">
-        <v>10.511988000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11">
-        <v>0.60530806000000004</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>0.60672959999999998</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>0.40722406</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>0.60585829999999996</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>0.38986418</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>0.62131625000000001</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>0.60610549999999996</v>
+        <v>6</v>
       </c>
       <c r="K11">
-        <v>0.61175597000000004</v>
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>0.52608319999999997</v>
+        <v>6</v>
       </c>
       <c r="M11">
-        <v>0.60557395000000003</v>
+        <v>6</v>
       </c>
       <c r="N11">
-        <v>0.51828969999999996</v>
+        <v>6</v>
       </c>
       <c r="O11">
-        <v>0.60281085999999995</v>
+        <v>6</v>
       </c>
       <c r="P11">
-        <v>0.60864339999999995</v>
+        <v>6</v>
       </c>
       <c r="Q11">
-        <v>0.60507619999999995</v>
+        <v>6</v>
       </c>
       <c r="R11">
-        <v>0.60420436</v>
+        <v>6</v>
       </c>
       <c r="S11">
-        <v>0.60536160000000006</v>
+        <v>6</v>
       </c>
       <c r="T11">
-        <v>0.60522880000000001</v>
+        <v>6</v>
       </c>
       <c r="U11">
-        <v>0.6053636</v>
+        <v>6</v>
       </c>
       <c r="V11">
-        <v>0.60534980000000005</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>11.5319</v>
+      </c>
+      <c r="C12">
+        <v>11.5158</v>
+      </c>
+      <c r="D12">
+        <v>4.9615</v>
+      </c>
+      <c r="E12">
+        <v>11.5367</v>
+      </c>
+      <c r="F12">
+        <v>4.7991000000000001</v>
+      </c>
+      <c r="G12">
+        <v>11.4735</v>
+      </c>
+      <c r="I12">
+        <v>11.539300000000001</v>
+      </c>
+      <c r="K12">
+        <v>11.552199999999999</v>
+      </c>
+      <c r="L12">
+        <v>8.3851999999999993</v>
+      </c>
+      <c r="M12">
+        <v>11.5342</v>
+      </c>
+      <c r="N12">
+        <v>8.2660999999999998</v>
+      </c>
+      <c r="O12">
+        <v>11.568199999999999</v>
+      </c>
+      <c r="P12">
+        <v>14.731299999999999</v>
+      </c>
+      <c r="Q12">
+        <v>11.529299999999999</v>
+      </c>
+      <c r="R12">
+        <v>14.725099999999999</v>
+      </c>
+      <c r="S12">
+        <v>11.532400000000001</v>
+      </c>
+      <c r="T12">
+        <v>11.523</v>
+      </c>
+      <c r="U12">
+        <v>11.5319</v>
+      </c>
+      <c r="V12">
+        <v>11.5237</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>10.088276</v>
+        <v>11.5319</v>
       </c>
       <c r="C13">
-        <v>10.172914499999999</v>
+        <v>11.532400000000001</v>
+      </c>
+      <c r="D13">
+        <v>9.8877000000000006</v>
       </c>
       <c r="E13">
-        <v>10.088552</v>
+        <v>11.537699999999999</v>
+      </c>
+      <c r="F13">
+        <v>9.5982000000000003</v>
       </c>
       <c r="G13">
-        <v>10.184378000000001</v>
+        <v>11.4985</v>
       </c>
       <c r="I13">
-        <v>10.088162000000001</v>
+        <v>11.540699999999999</v>
       </c>
       <c r="K13">
-        <v>10.125124</v>
+        <v>11.560499999999999</v>
       </c>
       <c r="L13">
-        <v>9.9728750000000002</v>
+        <v>11.1686</v>
       </c>
       <c r="M13">
-        <v>10.088305999999999</v>
+        <v>11.534700000000001</v>
       </c>
       <c r="N13">
-        <v>10.026384</v>
+        <v>11.0215</v>
       </c>
       <c r="O13">
-        <v>10.053661999999999</v>
+        <v>11.559900000000001</v>
       </c>
       <c r="P13">
-        <v>10.116463</v>
+        <v>11.7921</v>
       </c>
       <c r="Q13">
-        <v>10.088471999999999</v>
+        <v>11.5288</v>
       </c>
       <c r="R13">
-        <v>10.095207</v>
+        <v>11.780099999999999</v>
       </c>
       <c r="S13">
-        <v>10.088437000000001</v>
+        <v>11.532500000000001</v>
       </c>
       <c r="T13">
-        <v>10.088939</v>
+        <v>11.5345</v>
       </c>
       <c r="U13">
-        <v>10.088243</v>
+        <v>11.5319</v>
       </c>
       <c r="V13">
-        <v>10.089027</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>0.34060466</v>
-      </c>
-      <c r="C14">
-        <v>0.34060466</v>
-      </c>
-      <c r="D14">
-        <v>0.34060466</v>
-      </c>
-      <c r="E14">
-        <v>0.34060466</v>
-      </c>
-      <c r="F14">
-        <v>0.34060466</v>
-      </c>
-      <c r="G14">
-        <v>0.34060466</v>
-      </c>
-      <c r="H14">
-        <v>0.34060466</v>
-      </c>
-      <c r="I14">
-        <v>0.34060466</v>
-      </c>
-      <c r="J14">
-        <v>0.34060466</v>
-      </c>
-      <c r="K14">
-        <v>0.34060466</v>
-      </c>
-      <c r="L14">
-        <v>0.34060466</v>
-      </c>
-      <c r="M14">
-        <v>0.34060466</v>
-      </c>
-      <c r="N14">
-        <v>0.34060466</v>
-      </c>
-      <c r="O14">
-        <v>0.34060466</v>
-      </c>
-      <c r="P14">
-        <v>0.34060466</v>
-      </c>
-      <c r="Q14">
-        <v>0.34060466</v>
-      </c>
-      <c r="R14">
-        <v>0.34060466</v>
-      </c>
-      <c r="S14">
-        <v>0.34060466</v>
-      </c>
-      <c r="T14">
-        <v>0.34060466</v>
-      </c>
-      <c r="U14">
-        <v>0.34060466</v>
-      </c>
-      <c r="V14">
-        <v>0.34060466</v>
+        <v>11.5352</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>0.48480000000000001</v>
+        <v>10.511709</v>
       </c>
       <c r="C15">
-        <v>0.34060466</v>
+        <v>10.606191000000001</v>
+      </c>
+      <c r="D15">
+        <v>10.183984000000001</v>
       </c>
       <c r="E15">
-        <v>0.48480000000000001</v>
+        <v>10.512212</v>
+      </c>
+      <c r="F15">
+        <v>10.121859000000001</v>
       </c>
       <c r="G15">
-        <v>0.4884</v>
+        <v>10.623476999999999</v>
       </c>
       <c r="I15">
-        <v>0.48480000000000001</v>
+        <v>10.512638000000001</v>
       </c>
       <c r="K15">
-        <v>0.48620000000000002</v>
+        <v>10.546491</v>
       </c>
       <c r="L15">
-        <v>0.48049999999999998</v>
+        <v>10.453250000000001</v>
       </c>
       <c r="M15">
-        <v>0.48480000000000001</v>
+        <v>10.512064000000001</v>
       </c>
       <c r="N15">
-        <v>0.48249999999999998</v>
+        <v>10.442306500000001</v>
       </c>
       <c r="O15">
-        <v>0.48349999999999999</v>
+        <v>10.476487000000001</v>
       </c>
       <c r="P15">
-        <v>0.4859</v>
+        <v>10.4758</v>
       </c>
       <c r="Q15">
-        <v>0.48480000000000001</v>
+        <v>10.511231</v>
       </c>
       <c r="R15">
-        <v>0.48509999999999998</v>
+        <v>10.455652000000001</v>
       </c>
       <c r="S15">
-        <v>0.48480000000000001</v>
+        <v>10.511894</v>
       </c>
       <c r="T15">
-        <v>0.4849</v>
+        <v>10.511896</v>
       </c>
       <c r="U15">
-        <v>0.48480000000000001</v>
+        <v>10.511658000000001</v>
       </c>
       <c r="V15">
-        <v>0.4849</v>
+        <v>10.511988000000001</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>0.29007253</v>
+      </c>
+      <c r="C16">
+        <v>0.29007253</v>
+      </c>
+      <c r="D16">
+        <v>0.29007253</v>
+      </c>
+      <c r="E16">
+        <v>0.29007253</v>
+      </c>
+      <c r="F16">
+        <v>0.29007253</v>
+      </c>
+      <c r="G16">
+        <v>0.29007253</v>
+      </c>
+      <c r="H16">
+        <v>0.29007253</v>
+      </c>
+      <c r="I16">
+        <v>0.29007253</v>
+      </c>
+      <c r="J16">
+        <v>0.29007253</v>
+      </c>
+      <c r="K16">
+        <v>0.29007253</v>
+      </c>
+      <c r="L16">
+        <v>0.29007253</v>
+      </c>
+      <c r="M16">
+        <v>0.29007253</v>
+      </c>
+      <c r="N16">
+        <v>0.29007253</v>
+      </c>
+      <c r="O16">
+        <v>0.29007253</v>
+      </c>
+      <c r="P16">
+        <v>0.29007253</v>
+      </c>
+      <c r="Q16">
+        <v>0.29007253</v>
+      </c>
+      <c r="R16">
+        <v>0.29007253</v>
+      </c>
+      <c r="S16">
+        <v>0.29007253</v>
+      </c>
+      <c r="T16">
+        <v>0.29007253</v>
+      </c>
+      <c r="U16">
+        <v>0.29007253</v>
+      </c>
+      <c r="V16">
+        <v>0.29007253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>0.4864</v>
+      </c>
+      <c r="C17">
+        <v>0.4899</v>
+      </c>
+      <c r="D17">
+        <v>0.47410000000000002</v>
+      </c>
+      <c r="E17">
+        <v>0.4864</v>
+      </c>
+      <c r="F17">
+        <v>0.4718</v>
+      </c>
+      <c r="G17">
+        <v>0.49059999999999998</v>
+      </c>
+      <c r="I17">
+        <v>0.4864</v>
+      </c>
+      <c r="K17">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="L17">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="M17">
+        <v>0.4864</v>
+      </c>
+      <c r="N17">
+        <v>0.48380000000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.48509999999999998</v>
+      </c>
+      <c r="P17">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="Q17">
+        <v>0.4864</v>
+      </c>
+      <c r="R17">
+        <v>0.48430000000000001</v>
+      </c>
+      <c r="S17">
+        <v>0.4864</v>
+      </c>
+      <c r="T17">
+        <v>0.4864</v>
+      </c>
+      <c r="U17">
+        <v>0.4864</v>
+      </c>
+      <c r="V17">
+        <v>10.511988000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B18">
+        <v>0.60530806000000004</v>
+      </c>
+      <c r="C18">
+        <v>0.60672959999999998</v>
+      </c>
+      <c r="D18">
+        <v>0.40722406</v>
+      </c>
+      <c r="E18">
+        <v>0.60585829999999996</v>
+      </c>
+      <c r="F18">
+        <v>0.38986418</v>
+      </c>
+      <c r="G18">
+        <v>0.62131625000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.60610549999999996</v>
+      </c>
+      <c r="K18">
+        <v>0.61175597000000004</v>
+      </c>
+      <c r="L18">
+        <v>0.52608319999999997</v>
+      </c>
+      <c r="M18">
+        <v>0.60557395000000003</v>
+      </c>
+      <c r="N18">
+        <v>0.51828969999999996</v>
+      </c>
+      <c r="O18">
+        <v>0.60281085999999995</v>
+      </c>
+      <c r="P18">
+        <v>0.60864339999999995</v>
+      </c>
+      <c r="Q18">
+        <v>0.60507619999999995</v>
+      </c>
+      <c r="R18">
+        <v>0.60420436</v>
+      </c>
+      <c r="S18">
+        <v>0.60536160000000006</v>
+      </c>
+      <c r="T18">
+        <v>0.60522880000000001</v>
+      </c>
+      <c r="U18">
+        <v>0.6053636</v>
+      </c>
+      <c r="V18">
+        <v>0.60534980000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>3.2275999999999998</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <v>5.0797999999999996</v>
+      </c>
+      <c r="M19">
+        <v>6</v>
+      </c>
+      <c r="N19">
+        <v>5.0389999999999997</v>
+      </c>
+      <c r="O19">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <v>6</v>
+      </c>
+      <c r="R19">
+        <v>6</v>
+      </c>
+      <c r="S19">
+        <v>6</v>
+      </c>
+      <c r="T19">
+        <v>6</v>
+      </c>
+      <c r="U19">
+        <v>6</v>
+      </c>
+      <c r="V19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>6</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>6</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>6</v>
+      </c>
+      <c r="V20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>6.7760999999999996</v>
+      </c>
+      <c r="C21">
+        <v>6.8377999999999997</v>
+      </c>
+      <c r="D21">
+        <v>6.4893999999999998</v>
+      </c>
+      <c r="E21">
+        <v>6.7252000000000001</v>
+      </c>
+      <c r="F21">
+        <v>3.2275999999999998</v>
+      </c>
+      <c r="G21">
+        <v>6.8437999999999999</v>
+      </c>
+      <c r="I21">
+        <v>6.6997999999999998</v>
+      </c>
+      <c r="K21">
+        <v>6.7965999999999998</v>
+      </c>
+      <c r="L21">
+        <v>5.0797999999999996</v>
+      </c>
+      <c r="M21">
+        <v>6.7507000000000001</v>
+      </c>
+      <c r="N21">
+        <v>5.0389999999999997</v>
+      </c>
+      <c r="O21">
+        <v>6.7553000000000001</v>
+      </c>
+      <c r="P21">
+        <v>8.3989999999999991</v>
+      </c>
+      <c r="Q21">
+        <v>6.8014000000000001</v>
+      </c>
+      <c r="R21">
+        <v>8.4122000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>6.7760999999999996</v>
+      </c>
+      <c r="C22">
+        <v>6.8544999999999998</v>
+      </c>
+      <c r="D22">
+        <v>6.5061</v>
+      </c>
+      <c r="E22">
+        <v>6.7765000000000004</v>
+      </c>
+      <c r="F22">
+        <v>6.4551999999999996</v>
+      </c>
+      <c r="G22">
+        <v>6.8688000000000002</v>
+      </c>
+      <c r="I22">
+        <v>6.7769000000000004</v>
+      </c>
+      <c r="K22">
+        <v>6.8048999999999999</v>
+      </c>
+      <c r="L22">
+        <v>6.7278000000000002</v>
+      </c>
+      <c r="M22">
+        <v>6.7763999999999998</v>
+      </c>
+      <c r="N22">
+        <v>6.7187000000000001</v>
+      </c>
+      <c r="O22">
+        <v>6.7469999999999999</v>
+      </c>
+      <c r="P22">
+        <v>6.7464000000000004</v>
+      </c>
+      <c r="Q22">
+        <v>6.7756999999999996</v>
+      </c>
+      <c r="R22">
+        <v>6.7297000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>10.088276</v>
+      </c>
+      <c r="C24">
+        <v>10.172914499999999</v>
+      </c>
+      <c r="E24">
+        <v>10.088552</v>
+      </c>
+      <c r="G24">
+        <v>10.184378000000001</v>
+      </c>
+      <c r="I24">
+        <v>10.088162000000001</v>
+      </c>
+      <c r="K24">
+        <v>10.125124</v>
+      </c>
+      <c r="L24">
+        <v>9.9728750000000002</v>
+      </c>
+      <c r="M24">
+        <v>10.088305999999999</v>
+      </c>
+      <c r="N24">
+        <v>10.026384</v>
+      </c>
+      <c r="O24">
+        <v>10.053661999999999</v>
+      </c>
+      <c r="P24">
+        <v>10.116463</v>
+      </c>
+      <c r="Q24">
+        <v>10.088471999999999</v>
+      </c>
+      <c r="R24">
+        <v>10.095207</v>
+      </c>
+      <c r="S24">
+        <v>10.088437000000001</v>
+      </c>
+      <c r="T24">
+        <v>10.088939</v>
+      </c>
+      <c r="U24">
+        <v>10.088243</v>
+      </c>
+      <c r="V24">
+        <v>10.089027</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>0.34060466</v>
+      </c>
+      <c r="C25">
+        <v>0.34060466</v>
+      </c>
+      <c r="D25">
+        <v>0.34060466</v>
+      </c>
+      <c r="E25">
+        <v>0.34060466</v>
+      </c>
+      <c r="F25">
+        <v>0.34060466</v>
+      </c>
+      <c r="G25">
+        <v>0.34060466</v>
+      </c>
+      <c r="H25">
+        <v>0.34060466</v>
+      </c>
+      <c r="I25">
+        <v>0.34060466</v>
+      </c>
+      <c r="J25">
+        <v>0.34060466</v>
+      </c>
+      <c r="K25">
+        <v>0.34060466</v>
+      </c>
+      <c r="L25">
+        <v>0.34060466</v>
+      </c>
+      <c r="M25">
+        <v>0.34060466</v>
+      </c>
+      <c r="N25">
+        <v>0.34060466</v>
+      </c>
+      <c r="O25">
+        <v>0.34060466</v>
+      </c>
+      <c r="P25">
+        <v>0.34060466</v>
+      </c>
+      <c r="Q25">
+        <v>0.34060466</v>
+      </c>
+      <c r="R25">
+        <v>0.34060466</v>
+      </c>
+      <c r="S25">
+        <v>0.34060466</v>
+      </c>
+      <c r="T25">
+        <v>0.34060466</v>
+      </c>
+      <c r="U25">
+        <v>0.34060466</v>
+      </c>
+      <c r="V25">
+        <v>0.34060466</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="C26">
+        <v>0.48820000000000002</v>
+      </c>
+      <c r="E26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.4884</v>
+      </c>
+      <c r="I26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="K26">
+        <v>0.48620000000000002</v>
+      </c>
+      <c r="L26">
+        <v>0.48049999999999998</v>
+      </c>
+      <c r="M26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="N26">
+        <v>0.48249999999999998</v>
+      </c>
+      <c r="O26">
+        <v>0.48349999999999999</v>
+      </c>
+      <c r="P26">
+        <v>0.4859</v>
+      </c>
+      <c r="Q26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="R26">
+        <v>0.48509999999999998</v>
+      </c>
+      <c r="S26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="T26">
+        <v>0.4849</v>
+      </c>
+      <c r="U26">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="V26">
+        <v>0.4849</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
         <v>0.68085600000000002</v>
       </c>
-      <c r="C16">
+      <c r="C27">
         <v>0.64096624000000002</v>
       </c>
-      <c r="E16">
+      <c r="E27">
         <v>0.6803785</v>
       </c>
-      <c r="G16">
+      <c r="G27">
         <v>0.60257470000000002</v>
       </c>
-      <c r="I16">
+      <c r="I27">
         <v>0.68052029999999997</v>
       </c>
-      <c r="K16">
+      <c r="K27">
         <v>0.65760960000000002</v>
       </c>
-      <c r="L16">
+      <c r="L27">
         <v>0.62494479999999997</v>
       </c>
-      <c r="M16">
+      <c r="M27">
         <v>0.68055220000000005</v>
       </c>
-      <c r="N16">
+      <c r="N27">
         <v>0.60391843000000001</v>
       </c>
-      <c r="O16">
+      <c r="O27">
         <v>0.67636067</v>
       </c>
-      <c r="P16">
+      <c r="P27">
         <v>0.78299266000000001</v>
       </c>
-      <c r="Q16">
+      <c r="Q27">
         <v>0.68069259999999998</v>
       </c>
-      <c r="R16">
+      <c r="R27">
         <v>0.75873279999999999</v>
       </c>
-      <c r="S16">
+      <c r="S27">
         <v>0.68084513999999996</v>
       </c>
-      <c r="T16">
+      <c r="T27">
         <v>0.67894129999999997</v>
       </c>
-      <c r="U16">
+      <c r="U27">
         <v>0.68056333000000002</v>
       </c>
-      <c r="V16">
+      <c r="V27">
         <v>0.67868139999999999</v>
       </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding the excel sheet and the ros codes I used
</commit_message>
<xml_diff>
--- a/ROS_calculations.xlsx
+++ b/ROS_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/Hill_Runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E643DD7-2E8F-AA4C-A441-ED1512431DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E1DA7C-6B3F-6F48-8720-B3CA22F4B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="640" windowWidth="17280" windowHeight="21700" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
+    <workbookView xWindow="72960" yWindow="-7220" windowWidth="38400" windowHeight="21600" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C5D8E9-26BC-FC46-9670-57C49E39CB3F}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1625,6 +1626,18 @@
       <c r="R21">
         <v>8.4122000000000003</v>
       </c>
+      <c r="S21">
+        <v>6.7762000000000002</v>
+      </c>
+      <c r="T21">
+        <v>6.7695999999999996</v>
+      </c>
+      <c r="U21">
+        <v>6.7950999999999997</v>
+      </c>
+      <c r="V21">
+        <v>6.7763</v>
+      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1675,6 +1688,18 @@
       <c r="R22">
         <v>6.7297000000000002</v>
       </c>
+      <c r="S22">
+        <v>6.7763</v>
+      </c>
+      <c r="T22" s="2">
+        <v>6.7763</v>
+      </c>
+      <c r="U22">
+        <v>6.7760999999999996</v>
+      </c>
+      <c r="V22">
+        <v>6.7695999999999996</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1916,22 +1941,249 @@
       <c r="A28" t="s">
         <v>35</v>
       </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>6</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>6</v>
+      </c>
+      <c r="L28">
+        <v>4.8231000000000002</v>
+      </c>
+      <c r="M28">
+        <v>6</v>
+      </c>
+      <c r="N28">
+        <v>4.8121</v>
+      </c>
+      <c r="O28">
+        <v>6</v>
+      </c>
+      <c r="P28">
+        <v>6</v>
+      </c>
+      <c r="Q28">
+        <v>6</v>
+      </c>
+      <c r="R28">
+        <v>6</v>
+      </c>
+      <c r="S28">
+        <v>6</v>
+      </c>
+      <c r="T28">
+        <v>6</v>
+      </c>
+      <c r="U28">
+        <v>6</v>
+      </c>
+      <c r="V28">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>6</v>
+      </c>
+      <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="O29">
+        <v>6</v>
+      </c>
+      <c r="P29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>6</v>
+      </c>
+      <c r="R29">
+        <v>6</v>
+      </c>
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>6</v>
+      </c>
+      <c r="U29">
+        <v>6</v>
+      </c>
+      <c r="V29">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
+      <c r="B30">
+        <v>6.4665999999999997</v>
+      </c>
+      <c r="C30">
+        <v>6.5193000000000003</v>
+      </c>
+      <c r="E30">
+        <v>6.3959999999999999</v>
+      </c>
+      <c r="G30">
+        <v>6.5202999999999998</v>
+      </c>
+      <c r="I30">
+        <v>6.3602999999999996</v>
+      </c>
+      <c r="K30">
+        <v>6.4885000000000002</v>
+      </c>
+      <c r="L30">
+        <v>4.8231000000000002</v>
+      </c>
+      <c r="M30">
+        <v>6.4313000000000002</v>
+      </c>
+      <c r="N30">
+        <v>4.8121</v>
+      </c>
+      <c r="O30">
+        <v>6.4466999999999999</v>
+      </c>
+      <c r="P30">
+        <v>8.0684000000000005</v>
+      </c>
+      <c r="Q30">
+        <v>6.5022000000000002</v>
+      </c>
+      <c r="R30">
+        <v>8.0904000000000007</v>
+      </c>
+      <c r="S30">
+        <v>6.4667000000000003</v>
+      </c>
+      <c r="T30">
+        <v>6.4608999999999996</v>
+      </c>
+      <c r="U30">
+        <v>6.4664999999999999</v>
+      </c>
+      <c r="V30">
+        <v>6.4607999999999999</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1">
+        <v>6.4665999999999997</v>
+      </c>
+      <c r="C31">
+        <v>6.5358999999999998</v>
+      </c>
+      <c r="E31">
+        <v>6.4668999999999999</v>
+      </c>
+      <c r="G31">
+        <v>6.5453000000000001</v>
+      </c>
+      <c r="I31">
+        <v>6.4664999999999999</v>
+      </c>
+      <c r="K31">
+        <v>6.4968000000000004</v>
+      </c>
+      <c r="L31">
+        <v>6.3724999999999996</v>
+      </c>
+      <c r="M31">
+        <v>6.4667000000000003</v>
+      </c>
+      <c r="N31">
+        <v>6.4161000000000001</v>
+      </c>
+      <c r="O31">
+        <v>6.4383999999999997</v>
+      </c>
+      <c r="P31">
+        <v>6.4897</v>
+      </c>
+      <c r="Q31">
+        <v>6.4668000000000001</v>
+      </c>
+      <c r="R31">
+        <v>6.4722999999999997</v>
+      </c>
+      <c r="S31">
+        <v>6.4668000000000001</v>
+      </c>
+      <c r="T31">
+        <v>6.4672000000000001</v>
+      </c>
+      <c r="U31">
+        <v>6.4665999999999997</v>
+      </c>
+      <c r="V31">
+        <v>6.4672999999999998</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>

</xml_diff>

<commit_message>
Modifying the Rothermel code
</commit_message>
<xml_diff>
--- a/ROS_calculations.xlsx
+++ b/ROS_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/Hill_Runs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_Files/Hill_Runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E1DA7C-6B3F-6F48-8720-B3CA22F4B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A2729F9-697B-3344-80BF-7CC29C96F39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72960" yWindow="-7220" windowWidth="38400" windowHeight="21600" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{031D4DE6-AC10-0C46-90BE-D06C7BB4FFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C5D8E9-26BC-FC46-9670-57C49E39CB3F}">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1199,325 +1199,263 @@
         <v>11.5352</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>10.511709</v>
-      </c>
-      <c r="C15">
-        <v>10.606191000000001</v>
-      </c>
-      <c r="D15">
-        <v>10.183984000000001</v>
-      </c>
-      <c r="E15">
-        <v>10.512212</v>
-      </c>
-      <c r="F15">
-        <v>10.121859000000001</v>
-      </c>
-      <c r="G15">
-        <v>10.623476999999999</v>
-      </c>
-      <c r="I15">
-        <v>10.512638000000001</v>
-      </c>
-      <c r="K15">
-        <v>10.546491</v>
-      </c>
-      <c r="L15">
-        <v>10.453250000000001</v>
-      </c>
-      <c r="M15">
-        <v>10.512064000000001</v>
-      </c>
-      <c r="N15">
-        <v>10.442306500000001</v>
-      </c>
-      <c r="O15">
-        <v>10.476487000000001</v>
-      </c>
-      <c r="P15">
-        <v>10.4758</v>
-      </c>
-      <c r="Q15">
-        <v>10.511231</v>
-      </c>
-      <c r="R15">
-        <v>10.455652000000001</v>
-      </c>
-      <c r="S15">
-        <v>10.511894</v>
-      </c>
-      <c r="T15">
-        <v>10.511896</v>
-      </c>
-      <c r="U15">
-        <v>10.511658000000001</v>
-      </c>
-      <c r="V15">
-        <v>10.511988000000001</v>
-      </c>
-    </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>0.29007253</v>
+        <v>10.511709</v>
       </c>
       <c r="C16">
-        <v>0.29007253</v>
+        <v>10.606191000000001</v>
       </c>
       <c r="D16">
-        <v>0.29007253</v>
+        <v>10.183984000000001</v>
       </c>
       <c r="E16">
-        <v>0.29007253</v>
+        <v>10.512212</v>
       </c>
       <c r="F16">
-        <v>0.29007253</v>
+        <v>10.121859000000001</v>
       </c>
       <c r="G16">
-        <v>0.29007253</v>
-      </c>
-      <c r="H16">
-        <v>0.29007253</v>
+        <v>10.623476999999999</v>
       </c>
       <c r="I16">
-        <v>0.29007253</v>
-      </c>
-      <c r="J16">
-        <v>0.29007253</v>
+        <v>10.512638000000001</v>
       </c>
       <c r="K16">
-        <v>0.29007253</v>
+        <v>10.546491</v>
       </c>
       <c r="L16">
-        <v>0.29007253</v>
+        <v>10.453250000000001</v>
       </c>
       <c r="M16">
-        <v>0.29007253</v>
+        <v>10.512064000000001</v>
       </c>
       <c r="N16">
-        <v>0.29007253</v>
+        <v>10.442306500000001</v>
       </c>
       <c r="O16">
-        <v>0.29007253</v>
+        <v>10.476487000000001</v>
       </c>
       <c r="P16">
-        <v>0.29007253</v>
+        <v>10.4758</v>
       </c>
       <c r="Q16">
-        <v>0.29007253</v>
+        <v>10.511231</v>
       </c>
       <c r="R16">
-        <v>0.29007253</v>
+        <v>10.455652000000001</v>
       </c>
       <c r="S16">
-        <v>0.29007253</v>
+        <v>10.511894</v>
       </c>
       <c r="T16">
-        <v>0.29007253</v>
+        <v>10.511896</v>
       </c>
       <c r="U16">
-        <v>0.29007253</v>
+        <v>10.511658000000001</v>
       </c>
       <c r="V16">
-        <v>0.29007253</v>
+        <v>10.511988000000001</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="C17">
-        <v>0.4899</v>
+        <v>0.29007253</v>
       </c>
       <c r="D17">
-        <v>0.47410000000000002</v>
+        <v>0.29007253</v>
       </c>
       <c r="E17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="F17">
-        <v>0.4718</v>
+        <v>0.29007253</v>
       </c>
       <c r="G17">
-        <v>0.49059999999999998</v>
+        <v>0.29007253</v>
+      </c>
+      <c r="H17">
+        <v>0.29007253</v>
       </c>
       <c r="I17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
+      </c>
+      <c r="J17">
+        <v>0.29007253</v>
       </c>
       <c r="K17">
-        <v>0.48770000000000002</v>
+        <v>0.29007253</v>
       </c>
       <c r="L17">
-        <v>0.48770000000000002</v>
+        <v>0.29007253</v>
       </c>
       <c r="M17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="N17">
-        <v>0.48380000000000001</v>
+        <v>0.29007253</v>
       </c>
       <c r="O17">
-        <v>0.48509999999999998</v>
+        <v>0.29007253</v>
       </c>
       <c r="P17">
-        <v>0.48499999999999999</v>
+        <v>0.29007253</v>
       </c>
       <c r="Q17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="R17">
-        <v>0.48430000000000001</v>
+        <v>0.29007253</v>
       </c>
       <c r="S17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="T17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="U17">
-        <v>0.4864</v>
+        <v>0.29007253</v>
       </c>
       <c r="V17">
-        <v>10.511988000000001</v>
+        <v>0.29007253</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <v>0.60530806000000004</v>
+        <v>0.4864</v>
       </c>
       <c r="C18">
-        <v>0.60672959999999998</v>
+        <v>0.4899</v>
       </c>
       <c r="D18">
-        <v>0.40722406</v>
+        <v>0.47410000000000002</v>
       </c>
       <c r="E18">
-        <v>0.60585829999999996</v>
+        <v>0.4864</v>
       </c>
       <c r="F18">
-        <v>0.38986418</v>
+        <v>0.4718</v>
       </c>
       <c r="G18">
-        <v>0.62131625000000001</v>
+        <v>0.49059999999999998</v>
       </c>
       <c r="I18">
-        <v>0.60610549999999996</v>
+        <v>0.4864</v>
       </c>
       <c r="K18">
-        <v>0.61175597000000004</v>
+        <v>0.48770000000000002</v>
       </c>
       <c r="L18">
-        <v>0.52608319999999997</v>
+        <v>0.48770000000000002</v>
       </c>
       <c r="M18">
-        <v>0.60557395000000003</v>
+        <v>0.4864</v>
       </c>
       <c r="N18">
-        <v>0.51828969999999996</v>
+        <v>0.48380000000000001</v>
       </c>
       <c r="O18">
-        <v>0.60281085999999995</v>
+        <v>0.48509999999999998</v>
       </c>
       <c r="P18">
-        <v>0.60864339999999995</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="Q18">
-        <v>0.60507619999999995</v>
+        <v>0.4864</v>
       </c>
       <c r="R18">
-        <v>0.60420436</v>
+        <v>0.48430000000000001</v>
       </c>
       <c r="S18">
-        <v>0.60536160000000006</v>
+        <v>0.4864</v>
       </c>
       <c r="T18">
-        <v>0.60522880000000001</v>
+        <v>0.4864</v>
       </c>
       <c r="U18">
-        <v>0.6053636</v>
+        <v>0.4864</v>
       </c>
       <c r="V18">
-        <v>0.60534980000000005</v>
+        <v>10.511988000000001</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>0.60530806000000004</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>0.60672959999999998</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>0.40722406</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>0.60585829999999996</v>
       </c>
       <c r="F19">
-        <v>3.2275999999999998</v>
+        <v>0.38986418</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>0.62131625000000001</v>
       </c>
       <c r="I19">
-        <v>6</v>
+        <v>0.60610549999999996</v>
       </c>
       <c r="K19">
-        <v>6</v>
+        <v>0.61175597000000004</v>
       </c>
       <c r="L19">
-        <v>5.0797999999999996</v>
+        <v>0.52608319999999997</v>
       </c>
       <c r="M19">
-        <v>6</v>
+        <v>0.60557395000000003</v>
       </c>
       <c r="N19">
-        <v>5.0389999999999997</v>
+        <v>0.51828969999999996</v>
       </c>
       <c r="O19">
-        <v>6</v>
+        <v>0.60281085999999995</v>
       </c>
       <c r="P19">
-        <v>6</v>
+        <v>0.60864339999999995</v>
       </c>
       <c r="Q19">
-        <v>6</v>
+        <v>0.60507619999999995</v>
       </c>
       <c r="R19">
-        <v>6</v>
+        <v>0.60420436</v>
       </c>
       <c r="S19">
-        <v>6</v>
+        <v>0.60536160000000006</v>
       </c>
       <c r="T19">
-        <v>6</v>
+        <v>0.60522880000000001</v>
       </c>
       <c r="U19">
-        <v>6</v>
+        <v>0.6053636</v>
       </c>
       <c r="V19">
-        <v>6</v>
+        <v>0.60534980000000005</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1532,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>3.2275999999999998</v>
       </c>
       <c r="G20">
         <v>6</v>
@@ -1544,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="L20">
-        <v>6</v>
+        <v>5.0797999999999996</v>
       </c>
       <c r="M20">
         <v>6</v>
       </c>
       <c r="N20">
-        <v>6</v>
+        <v>5.0389999999999997</v>
       </c>
       <c r="O20">
         <v>6</v>
@@ -1579,661 +1517,720 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21">
-        <v>6.7760999999999996</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>6.8377999999999997</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>6.4893999999999998</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>6.7252000000000001</v>
+        <v>6</v>
       </c>
       <c r="F21">
-        <v>3.2275999999999998</v>
+        <v>6</v>
       </c>
       <c r="G21">
-        <v>6.8437999999999999</v>
+        <v>6</v>
       </c>
       <c r="I21">
-        <v>6.6997999999999998</v>
+        <v>6</v>
       </c>
       <c r="K21">
-        <v>6.7965999999999998</v>
+        <v>6</v>
       </c>
       <c r="L21">
-        <v>5.0797999999999996</v>
+        <v>6</v>
       </c>
       <c r="M21">
-        <v>6.7507000000000001</v>
+        <v>6</v>
       </c>
       <c r="N21">
-        <v>5.0389999999999997</v>
+        <v>6</v>
       </c>
       <c r="O21">
-        <v>6.7553000000000001</v>
+        <v>6</v>
       </c>
       <c r="P21">
-        <v>8.3989999999999991</v>
+        <v>6</v>
       </c>
       <c r="Q21">
-        <v>6.8014000000000001</v>
+        <v>6</v>
       </c>
       <c r="R21">
-        <v>8.4122000000000003</v>
+        <v>6</v>
       </c>
       <c r="S21">
-        <v>6.7762000000000002</v>
+        <v>6</v>
       </c>
       <c r="T21">
-        <v>6.7695999999999996</v>
+        <v>6</v>
       </c>
       <c r="U21">
-        <v>6.7950999999999997</v>
+        <v>6</v>
       </c>
       <c r="V21">
-        <v>6.7763</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>6.7760999999999996</v>
       </c>
       <c r="C22">
+        <v>6.8377999999999997</v>
+      </c>
+      <c r="D22">
+        <v>6.4893999999999998</v>
+      </c>
+      <c r="E22">
+        <v>6.7252000000000001</v>
+      </c>
+      <c r="F22">
+        <v>3.2275999999999998</v>
+      </c>
+      <c r="G22">
+        <v>6.8437999999999999</v>
+      </c>
+      <c r="I22">
+        <v>6.6997999999999998</v>
+      </c>
+      <c r="K22">
+        <v>6.7965999999999998</v>
+      </c>
+      <c r="L22">
+        <v>5.0797999999999996</v>
+      </c>
+      <c r="M22">
+        <v>6.7507000000000001</v>
+      </c>
+      <c r="N22">
+        <v>5.0389999999999997</v>
+      </c>
+      <c r="O22">
+        <v>6.7553000000000001</v>
+      </c>
+      <c r="P22">
+        <v>8.3989999999999991</v>
+      </c>
+      <c r="Q22">
+        <v>6.8014000000000001</v>
+      </c>
+      <c r="R22">
+        <v>8.4122000000000003</v>
+      </c>
+      <c r="S22">
+        <v>6.7762000000000002</v>
+      </c>
+      <c r="T22">
+        <v>6.7695999999999996</v>
+      </c>
+      <c r="U22">
+        <v>6.7950999999999997</v>
+      </c>
+      <c r="V22">
+        <v>6.7763</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>6.7760999999999996</v>
+      </c>
+      <c r="C23">
         <v>6.8544999999999998</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>6.5061</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>6.7765000000000004</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>6.4551999999999996</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>6.8688000000000002</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>6.7769000000000004</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>6.8048999999999999</v>
       </c>
-      <c r="L22">
+      <c r="L23">
         <v>6.7278000000000002</v>
       </c>
-      <c r="M22">
+      <c r="M23">
         <v>6.7763999999999998</v>
       </c>
-      <c r="N22">
+      <c r="N23">
         <v>6.7187000000000001</v>
       </c>
-      <c r="O22">
+      <c r="O23">
         <v>6.7469999999999999</v>
       </c>
-      <c r="P22">
+      <c r="P23">
         <v>6.7464000000000004</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <v>6.7756999999999996</v>
       </c>
-      <c r="R22">
+      <c r="R23">
         <v>6.7297000000000002</v>
       </c>
-      <c r="S22">
+      <c r="S23">
         <v>6.7763</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T23" s="2">
         <v>6.7763</v>
       </c>
-      <c r="U22">
+      <c r="U23">
         <v>6.7760999999999996</v>
       </c>
-      <c r="V22">
+      <c r="V23">
         <v>6.7695999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>10.088276</v>
-      </c>
-      <c r="C24">
-        <v>10.172914499999999</v>
-      </c>
-      <c r="E24">
-        <v>10.088552</v>
-      </c>
-      <c r="G24">
-        <v>10.184378000000001</v>
-      </c>
-      <c r="I24">
-        <v>10.088162000000001</v>
-      </c>
-      <c r="K24">
-        <v>10.125124</v>
-      </c>
-      <c r="L24">
-        <v>9.9728750000000002</v>
-      </c>
-      <c r="M24">
-        <v>10.088305999999999</v>
-      </c>
-      <c r="N24">
-        <v>10.026384</v>
-      </c>
-      <c r="O24">
-        <v>10.053661999999999</v>
-      </c>
-      <c r="P24">
-        <v>10.116463</v>
-      </c>
-      <c r="Q24">
-        <v>10.088471999999999</v>
-      </c>
-      <c r="R24">
-        <v>10.095207</v>
-      </c>
-      <c r="S24">
-        <v>10.088437000000001</v>
-      </c>
-      <c r="T24">
-        <v>10.088939</v>
-      </c>
-      <c r="U24">
-        <v>10.088243</v>
-      </c>
-      <c r="V24">
-        <v>10.089027</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>0.34060466</v>
-      </c>
-      <c r="C25">
-        <v>0.34060466</v>
-      </c>
-      <c r="D25">
-        <v>0.34060466</v>
-      </c>
-      <c r="E25">
-        <v>0.34060466</v>
-      </c>
-      <c r="F25">
-        <v>0.34060466</v>
-      </c>
-      <c r="G25">
-        <v>0.34060466</v>
-      </c>
-      <c r="H25">
-        <v>0.34060466</v>
-      </c>
-      <c r="I25">
-        <v>0.34060466</v>
-      </c>
-      <c r="J25">
-        <v>0.34060466</v>
-      </c>
-      <c r="K25">
-        <v>0.34060466</v>
-      </c>
-      <c r="L25">
-        <v>0.34060466</v>
-      </c>
-      <c r="M25">
-        <v>0.34060466</v>
-      </c>
-      <c r="N25">
-        <v>0.34060466</v>
-      </c>
-      <c r="O25">
-        <v>0.34060466</v>
-      </c>
-      <c r="P25">
-        <v>0.34060466</v>
-      </c>
-      <c r="Q25">
-        <v>0.34060466</v>
-      </c>
-      <c r="R25">
-        <v>0.34060466</v>
-      </c>
-      <c r="S25">
-        <v>0.34060466</v>
-      </c>
-      <c r="T25">
-        <v>0.34060466</v>
-      </c>
-      <c r="U25">
-        <v>0.34060466</v>
-      </c>
-      <c r="V25">
-        <v>0.34060466</v>
-      </c>
+      <c r="T24" s="2"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26">
-        <v>0.48480000000000001</v>
+        <v>10.088276</v>
       </c>
       <c r="C26">
-        <v>0.48820000000000002</v>
+        <v>10.172914499999999</v>
       </c>
       <c r="E26">
-        <v>0.48480000000000001</v>
+        <v>10.088552</v>
       </c>
       <c r="G26">
-        <v>0.4884</v>
+        <v>10.184378000000001</v>
       </c>
       <c r="I26">
-        <v>0.48480000000000001</v>
+        <v>10.088162000000001</v>
       </c>
       <c r="K26">
-        <v>0.48620000000000002</v>
+        <v>10.125124</v>
       </c>
       <c r="L26">
-        <v>0.48049999999999998</v>
+        <v>9.9728750000000002</v>
       </c>
       <c r="M26">
-        <v>0.48480000000000001</v>
+        <v>10.088305999999999</v>
       </c>
       <c r="N26">
-        <v>0.48249999999999998</v>
+        <v>10.026384</v>
       </c>
       <c r="O26">
-        <v>0.48349999999999999</v>
+        <v>10.053661999999999</v>
       </c>
       <c r="P26">
-        <v>0.4859</v>
+        <v>10.116463</v>
       </c>
       <c r="Q26">
-        <v>0.48480000000000001</v>
+        <v>10.088471999999999</v>
       </c>
       <c r="R26">
-        <v>0.48509999999999998</v>
+        <v>10.095207</v>
       </c>
       <c r="S26">
-        <v>0.48480000000000001</v>
+        <v>10.088437000000001</v>
       </c>
       <c r="T26">
-        <v>0.4849</v>
+        <v>10.088939</v>
       </c>
       <c r="U26">
-        <v>0.48480000000000001</v>
+        <v>10.088243</v>
       </c>
       <c r="V26">
-        <v>0.4849</v>
+        <v>10.089027</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B27">
-        <v>0.68085600000000002</v>
+        <v>0.34060466</v>
       </c>
       <c r="C27">
-        <v>0.64096624000000002</v>
+        <v>0.34060466</v>
+      </c>
+      <c r="D27">
+        <v>0.34060466</v>
       </c>
       <c r="E27">
-        <v>0.6803785</v>
+        <v>0.34060466</v>
+      </c>
+      <c r="F27">
+        <v>0.34060466</v>
       </c>
       <c r="G27">
-        <v>0.60257470000000002</v>
+        <v>0.34060466</v>
+      </c>
+      <c r="H27">
+        <v>0.34060466</v>
       </c>
       <c r="I27">
-        <v>0.68052029999999997</v>
+        <v>0.34060466</v>
+      </c>
+      <c r="J27">
+        <v>0.34060466</v>
       </c>
       <c r="K27">
-        <v>0.65760960000000002</v>
+        <v>0.34060466</v>
       </c>
       <c r="L27">
-        <v>0.62494479999999997</v>
+        <v>0.34060466</v>
       </c>
       <c r="M27">
-        <v>0.68055220000000005</v>
+        <v>0.34060466</v>
       </c>
       <c r="N27">
-        <v>0.60391843000000001</v>
+        <v>0.34060466</v>
       </c>
       <c r="O27">
-        <v>0.67636067</v>
+        <v>0.34060466</v>
       </c>
       <c r="P27">
-        <v>0.78299266000000001</v>
+        <v>0.34060466</v>
       </c>
       <c r="Q27">
-        <v>0.68069259999999998</v>
+        <v>0.34060466</v>
       </c>
       <c r="R27">
-        <v>0.75873279999999999</v>
+        <v>0.34060466</v>
       </c>
       <c r="S27">
-        <v>0.68084513999999996</v>
+        <v>0.34060466</v>
       </c>
       <c r="T27">
-        <v>0.67894129999999997</v>
+        <v>0.34060466</v>
       </c>
       <c r="U27">
-        <v>0.68056333000000002</v>
+        <v>0.34060466</v>
       </c>
       <c r="V27">
-        <v>0.67868139999999999</v>
+        <v>0.34060466</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="C28">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
+        <v>0.48820000000000002</v>
       </c>
       <c r="E28">
-        <v>6</v>
-      </c>
-      <c r="F28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="G28">
-        <v>6</v>
-      </c>
-      <c r="H28">
-        <v>6</v>
+        <v>0.4884</v>
       </c>
       <c r="I28">
-        <v>6</v>
-      </c>
-      <c r="J28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="K28">
-        <v>6</v>
+        <v>0.48620000000000002</v>
       </c>
       <c r="L28">
-        <v>4.8231000000000002</v>
+        <v>0.48049999999999998</v>
       </c>
       <c r="M28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="N28">
-        <v>4.8121</v>
+        <v>0.48249999999999998</v>
       </c>
       <c r="O28">
-        <v>6</v>
+        <v>0.48349999999999999</v>
       </c>
       <c r="P28">
-        <v>6</v>
+        <v>0.4859</v>
       </c>
       <c r="Q28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="R28">
-        <v>6</v>
+        <v>0.48509999999999998</v>
       </c>
       <c r="S28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="T28">
-        <v>6</v>
+        <v>0.4849</v>
       </c>
       <c r="U28">
-        <v>6</v>
+        <v>0.48480000000000001</v>
       </c>
       <c r="V28">
-        <v>6</v>
+        <v>0.4849</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>0.68085600000000002</v>
       </c>
       <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
+        <v>0.64096624000000002</v>
       </c>
       <c r="E29">
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
+        <v>0.6803785</v>
       </c>
       <c r="G29">
-        <v>6</v>
-      </c>
-      <c r="H29">
-        <v>6</v>
+        <v>0.60257470000000002</v>
       </c>
       <c r="I29">
-        <v>6</v>
-      </c>
-      <c r="J29">
-        <v>6</v>
+        <v>0.68052029999999997</v>
       </c>
       <c r="K29">
-        <v>6</v>
+        <v>0.65760960000000002</v>
       </c>
       <c r="L29">
-        <v>6</v>
+        <v>0.62494479999999997</v>
       </c>
       <c r="M29">
-        <v>6</v>
+        <v>0.68055220000000005</v>
       </c>
       <c r="N29">
-        <v>6</v>
+        <v>0.60391843000000001</v>
       </c>
       <c r="O29">
-        <v>6</v>
+        <v>0.67636067</v>
       </c>
       <c r="P29">
-        <v>6</v>
+        <v>0.78299266000000001</v>
       </c>
       <c r="Q29">
-        <v>6</v>
+        <v>0.68069259999999998</v>
       </c>
       <c r="R29">
-        <v>6</v>
+        <v>0.75873279999999999</v>
       </c>
       <c r="S29">
-        <v>6</v>
+        <v>0.68084513999999996</v>
       </c>
       <c r="T29">
-        <v>6</v>
+        <v>0.67894129999999997</v>
       </c>
       <c r="U29">
-        <v>6</v>
+        <v>0.68056333000000002</v>
       </c>
       <c r="V29">
-        <v>6</v>
+        <v>0.67868139999999999</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>6.4665999999999997</v>
+        <v>6</v>
       </c>
       <c r="C30">
-        <v>6.5193000000000003</v>
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>6.3959999999999999</v>
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
       </c>
       <c r="G30">
-        <v>6.5202999999999998</v>
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
       </c>
       <c r="I30">
-        <v>6.3602999999999996</v>
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
       </c>
       <c r="K30">
-        <v>6.4885000000000002</v>
+        <v>6</v>
       </c>
       <c r="L30">
         <v>4.8231000000000002</v>
       </c>
       <c r="M30">
-        <v>6.4313000000000002</v>
+        <v>6</v>
       </c>
       <c r="N30">
         <v>4.8121</v>
       </c>
       <c r="O30">
-        <v>6.4466999999999999</v>
+        <v>6</v>
       </c>
       <c r="P30">
-        <v>8.0684000000000005</v>
+        <v>6</v>
       </c>
       <c r="Q30">
-        <v>6.5022000000000002</v>
+        <v>6</v>
       </c>
       <c r="R30">
-        <v>8.0904000000000007</v>
+        <v>6</v>
       </c>
       <c r="S30">
-        <v>6.4667000000000003</v>
+        <v>6</v>
       </c>
       <c r="T30">
-        <v>6.4608999999999996</v>
+        <v>6</v>
       </c>
       <c r="U30">
-        <v>6.4664999999999999</v>
+        <v>6</v>
       </c>
       <c r="V30">
-        <v>6.4607999999999999</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>6</v>
+      </c>
+      <c r="M31">
+        <v>6</v>
+      </c>
+      <c r="N31">
+        <v>6</v>
+      </c>
+      <c r="O31">
+        <v>6</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
+      <c r="Q31">
+        <v>6</v>
+      </c>
+      <c r="R31">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <v>6</v>
+      </c>
+      <c r="T31">
+        <v>6</v>
+      </c>
+      <c r="U31">
+        <v>6</v>
+      </c>
+      <c r="V31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32">
+        <v>6.4665999999999997</v>
+      </c>
+      <c r="C32">
+        <v>6.5193000000000003</v>
+      </c>
+      <c r="E32">
+        <v>6.3959999999999999</v>
+      </c>
+      <c r="G32">
+        <v>6.5202999999999998</v>
+      </c>
+      <c r="I32">
+        <v>6.3602999999999996</v>
+      </c>
+      <c r="K32">
+        <v>6.4885000000000002</v>
+      </c>
+      <c r="L32">
+        <v>4.8231000000000002</v>
+      </c>
+      <c r="M32">
+        <v>6.4313000000000002</v>
+      </c>
+      <c r="N32">
+        <v>4.8121</v>
+      </c>
+      <c r="O32">
+        <v>6.4466999999999999</v>
+      </c>
+      <c r="P32">
+        <v>8.0684000000000005</v>
+      </c>
+      <c r="Q32">
+        <v>6.5022000000000002</v>
+      </c>
+      <c r="R32">
+        <v>8.0904000000000007</v>
+      </c>
+      <c r="S32">
+        <v>6.4667000000000003</v>
+      </c>
+      <c r="T32">
+        <v>6.4608999999999996</v>
+      </c>
+      <c r="U32">
+        <v>6.4664999999999999</v>
+      </c>
+      <c r="V32">
+        <v>6.4607999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B33" s="1">
         <v>6.4665999999999997</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <v>6.5358999999999998</v>
       </c>
-      <c r="E31">
+      <c r="E33">
         <v>6.4668999999999999</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <v>6.5453000000000001</v>
       </c>
-      <c r="I31">
+      <c r="I33">
         <v>6.4664999999999999</v>
       </c>
-      <c r="K31">
+      <c r="K33">
         <v>6.4968000000000004</v>
       </c>
-      <c r="L31">
+      <c r="L33">
         <v>6.3724999999999996</v>
       </c>
-      <c r="M31">
+      <c r="M33">
         <v>6.4667000000000003</v>
       </c>
-      <c r="N31">
+      <c r="N33">
         <v>6.4161000000000001</v>
       </c>
-      <c r="O31">
+      <c r="O33">
         <v>6.4383999999999997</v>
       </c>
-      <c r="P31">
+      <c r="P33">
         <v>6.4897</v>
       </c>
-      <c r="Q31">
+      <c r="Q33">
         <v>6.4668000000000001</v>
       </c>
-      <c r="R31">
+      <c r="R33">
         <v>6.4722999999999997</v>
       </c>
-      <c r="S31">
+      <c r="S33">
         <v>6.4668000000000001</v>
       </c>
-      <c r="T31">
+      <c r="T33">
         <v>6.4672000000000001</v>
       </c>
-      <c r="U31">
+      <c r="U33">
         <v>6.4665999999999997</v>
       </c>
-      <c r="V31">
+      <c r="V33">
         <v>6.4672999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
@@ -2244,6 +2241,12 @@
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>